<commit_message>
Tab field filter repository - added basic insert.
</commit_message>
<xml_diff>
--- a/input_file.xlsx
+++ b/input_file.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
   <si>
     <t xml:space="preserve">Tab name</t>
   </si>
@@ -29,9 +29,6 @@
     <t xml:space="preserve">Filter name</t>
   </si>
   <si>
-    <t xml:space="preserve">Field name</t>
-  </si>
-  <si>
     <t xml:space="preserve">Variant column name</t>
   </si>
   <si>
@@ -50,18 +47,12 @@
     <t xml:space="preserve">Filter 11</t>
   </si>
   <si>
-    <t xml:space="preserve">Field 111</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chrom</t>
   </si>
   <si>
     <t xml:space="preserve">Greater than</t>
   </si>
   <si>
-    <t xml:space="preserve">Field 112</t>
-  </si>
-  <si>
     <t xml:space="preserve">Position</t>
   </si>
   <si>
@@ -71,9 +62,6 @@
     <t xml:space="preserve">Filter 12</t>
   </si>
   <si>
-    <t xml:space="preserve">Field 121</t>
-  </si>
-  <si>
     <t xml:space="preserve">Reference</t>
   </si>
   <si>
@@ -83,15 +71,9 @@
     <t xml:space="preserve">C</t>
   </si>
   <si>
-    <t xml:space="preserve">Field 122</t>
-  </si>
-  <si>
     <t xml:space="preserve">Less than</t>
   </si>
   <si>
-    <t xml:space="preserve">Field 123</t>
-  </si>
-  <si>
     <t xml:space="preserve">Allele Number</t>
   </si>
   <si>
@@ -101,31 +83,16 @@
     <t xml:space="preserve">Filter 21</t>
   </si>
   <si>
-    <t xml:space="preserve">Field 211</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Field 212</t>
-  </si>
-  <si>
     <t xml:space="preserve">Filter 22</t>
   </si>
   <si>
-    <t xml:space="preserve">Field 221</t>
-  </si>
-  <si>
     <t xml:space="preserve">G</t>
   </si>
   <si>
-    <t xml:space="preserve">Field 222</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tab 3</t>
   </si>
   <si>
     <t xml:space="preserve">Filter 31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Field 331</t>
   </si>
   <si>
     <t xml:space="preserve">Relation values:</t>
@@ -331,18 +298,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.0102040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.0102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -364,211 +331,178 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="0" t="n">
+      <c r="E2" s="0" t="n">
         <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>8</v>
-      </c>
       <c r="C3" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E5" s="0" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="n">
         <v>42920</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="E7" s="0" t="n">
         <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E10" s="0" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1" t="n">
         <v>23686</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E11" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D11" type="list">
       <formula1>"Equals,Greater,Greater than,Less,Less than,Contains"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D11" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2:C11" type="list">
       <formula1>Sheet2!$D$2:$D$36</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -601,203 +535,203 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="0" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="0" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="0" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D11" s="0" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="0" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="0" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="0" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D15" s="0" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D16" s="0" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="0" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="0" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D19" s="0" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D20" s="0" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="0" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D22" s="0" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D23" s="0" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="0" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D25" s="0" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D26" s="0" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D27" s="0" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D28" s="0" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D29" s="0" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D30" s="0" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D31" s="0" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D32" s="0" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D33" s="0" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D34" s="0" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D35" s="0" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D36" s="0" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>